<commit_message>
in progress fix site same species
</commit_message>
<xml_diff>
--- a/0_setup_variables.xlsx
+++ b/0_setup_variables.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eilishmcmaster/Documents/ReCER_base_analysis_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E3C4D5-B370-DD41-BE85-0BFA4BBDE116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5519A92-8E6B-3B47-9CF5-F617C6A0FFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1080" windowWidth="38400" windowHeight="21600" xr2:uid="{60476AE5-51B8-3F47-9EEF-7B1574A266D9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{60476AE5-51B8-3F47-9EEF-7B1574A266D9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>species</t>
   </si>
@@ -62,15 +63,15 @@
     <t>site</t>
   </si>
   <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
     <t>notes</t>
   </si>
   <si>
-    <t>Variable</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>species_col_name</t>
   </si>
   <si>
@@ -87,6 +88,15 @@
   </si>
   <si>
     <t>downsample_pops</t>
+  </si>
+  <si>
+    <t>PersHirs</t>
+  </si>
+  <si>
+    <t>DPers21-6117</t>
+  </si>
+  <si>
+    <t>/Users/eilishmcmaster/Documents/ReCER_base_analysis_pipeline/PersHirs/meta/samples-2023-11-07_213926/Tissue-2023-11-07_213926.csv</t>
   </si>
 </sst>
 </file>
@@ -445,11 +455,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B4CFC2-A468-E24A-B5E2-9A35D4D9FA2D}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="124" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A068400-0900-C540-8ABF-E66849164AEC}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,13 +553,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added sample vs locus missingness
</commit_message>
<xml_diff>
--- a/0_setup_variables.xlsx
+++ b/0_setup_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eilishmcmaster/Documents/ReCER_base_analysis_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7242C7-A05A-C44A-A514-FD19F79265FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBD04C2-AB7F-E846-A4D9-4FC48136F0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1080" windowWidth="38400" windowHeight="21600" xr2:uid="{60476AE5-51B8-3F47-9EEF-7B1574A266D9}"/>
+    <workbookView xWindow="-38400" yWindow="-580" windowWidth="38400" windowHeight="21100" xr2:uid="{60476AE5-51B8-3F47-9EEF-7B1574A266D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>species</t>
   </si>
@@ -136,6 +136,18 @@
   </si>
   <si>
     <t>/Users/eilishmcmaster/Documents/ReCER_base_analysis_pipeline/TeucJunc/meta/samples-2023-11-10_100804/Tissue-2023-11-10_100804.csv</t>
+  </si>
+  <si>
+    <t>locus_missingness</t>
+  </si>
+  <si>
+    <t>sample_missingness</t>
+  </si>
+  <si>
+    <t>remove samples with missingness higher than this value</t>
+  </si>
+  <si>
+    <t>remove loci with missingness higher than this value</t>
   </si>
 </sst>
 </file>
@@ -512,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A068400-0900-C540-8ABF-E66849164AEC}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -626,34 +638,45 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B10" s="3">
         <v>0.4</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B11" s="3">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B13" s="3">
         <v>0.4</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added comments to splitstree
</commit_message>
<xml_diff>
--- a/0_setup_variables.xlsx
+++ b/0_setup_variables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eilishmcmaster/Documents/ReCER_base_analysis_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8E4206-4EF1-0D4E-A691-FB21A3F2D17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417CCEE5-0982-1348-92C1-B6C50E633B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{60476AE5-51B8-3F47-9EEF-7B1574A266D9}"/>
   </bookViews>
@@ -227,9 +227,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -267,7 +267,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -373,7 +373,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -515,7 +515,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -526,7 +526,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>